<commit_message>
Analyse des camps #29
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_camps.xlsx
+++ b/fichiers/conf/modele_camps.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55AE6E31-D7CB-4116-A544-52DB4598A985}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D588BCBC-2366-42F1-91AA-4DE5090E6443}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5940" yWindow="4230" windowWidth="21600" windowHeight="11250" xr2:uid="{8F248F90-B83D-4D26-B898-E0FFBFE01865}"/>
+    <workbookView xWindow="2265" yWindow="1560" windowWidth="27075" windowHeight="13650" activeTab="1" xr2:uid="{8F248F90-B83D-4D26-B898-E0FFBFE01865}"/>
   </bookViews>
   <sheets>
     <sheet name="camps" sheetId="1" r:id="rId1"/>
+    <sheet name="camps (maitrises)" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">camps!$A$1:$E$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">camps!$A$1:$H$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'camps (maitrises)'!$A$1:$D$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Unité</t>
   </si>
@@ -63,10 +65,43 @@
     <t>${camp.Jeunes}</t>
   </si>
   <si>
-    <t>Structure</t>
-  </si>
-  <si>
-    <t>${camp.Structure}</t>
+    <t>Code Groupe</t>
+  </si>
+  <si>
+    <t>Code Structure</t>
+  </si>
+  <si>
+    <t>${camp.unite.codegroupe}</t>
+  </si>
+  <si>
+    <t>${camp.unite.codestructure}</t>
+  </si>
+  <si>
+    <t>${camp.unite.nom}</t>
+  </si>
+  <si>
+    <t>Nb de chefs</t>
+  </si>
+  <si>
+    <t>${camp.Chefs}</t>
+  </si>
+  <si>
+    <t>&lt;jt:forEach items="${maitrises}" var="maitrise"&gt;</t>
+  </si>
+  <si>
+    <t>${maitrise.chef.nom}</t>
+  </si>
+  <si>
+    <t>${maitrise.chef.unite}</t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>Prénom</t>
+  </si>
+  <si>
+    <t>${maitrise.chef.prenom}</t>
   </si>
 </sst>
 </file>
@@ -117,7 +152,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -140,11 +175,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -159,11 +205,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -494,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67877FCE-0AFF-4AEB-B17A-D7414C418278}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,12 +580,14 @@
     <col min="1" max="1" width="18.140625" customWidth="1"/>
     <col min="2" max="2" width="74.5703125" customWidth="1"/>
     <col min="3" max="3" width="39.140625" customWidth="1"/>
-    <col min="4" max="4" width="49.7109375" customWidth="1"/>
-    <col min="5" max="10" width="19.42578125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="49.7109375" customWidth="1"/>
+    <col min="7" max="12" width="19.42578125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -520,19 +597,27 @@
       <c r="C1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="H1" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -542,24 +627,101 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="H2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="1"/>
+      <c r="N2" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="L2">
+  <autoFilter ref="A1:H2" xr:uid="{356B0EE0-0B5E-40EA-B9A9-555743EA321E}"/>
+  <conditionalFormatting sqref="N2">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2">
+    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"Non"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED25F9A8-E5E2-4E09-A2E0-FD92163DE898}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="44.140625" customWidth="1"/>
+    <col min="3" max="3" width="41" customWidth="1"/>
+    <col min="4" max="4" width="49.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D2" xr:uid="{356B0EE0-0B5E-40EA-B9A9-555743EA321E}"/>
+  <conditionalFormatting sqref="G2">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2">
+  <conditionalFormatting sqref="F2">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>

</xml_diff>